<commit_message>
hien thi du lieu ra formHanhKiem formHocLuc
</commit_message>
<xml_diff>
--- a/Testing/File ghi lỗi khi Test - QLHSGV.xlsx
+++ b/Testing/File ghi lỗi khi Test - QLHSGV.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thg60\OneDrive\Desktop\QLHS\QLHSGV\Testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AF5026-BBBE-4242-A3EC-8EA681187300}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="23256" windowHeight="12792"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,8 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +156,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -196,7 +210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,9 +242,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,6 +294,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,25 +487,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="5"/>
-    <col min="2" max="2" width="90.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="5"/>
+    <col min="2" max="2" width="90.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="13.8">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -475,7 +525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.8">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -495,7 +545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -509,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.8">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -523,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -537,12 +587,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8">
+    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -554,24 +604,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chỉnh sửa cập nhật quy định
Đã có thể cập nhật thông tin mới lên dtb
</commit_message>
<xml_diff>
--- a/Testing/File ghi lỗi khi Test - QLHSGV.xlsx
+++ b/Testing/File ghi lỗi khi Test - QLHSGV.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thg60\OneDrive\Desktop\QLHS\QLHSGV\Testing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AF5026-BBBE-4242-A3EC-8EA681187300}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Tùng</t>
   </si>
   <si>
-    <t>Việt</t>
-  </si>
-  <si>
     <t>Vấn đề</t>
   </si>
   <si>
@@ -48,38 +39,20 @@
     <t>STT</t>
   </si>
   <si>
-    <t>Xuất hiện bảng thông báo lỗi kết nối trước khi nhập tên server</t>
-  </si>
-  <si>
-    <t>Nhấn nút 'Test Connection' (trước khi nhập tên server) vẫn xuất hiện bảng "Kết nối thành công"</t>
-  </si>
-  <si>
-    <t>Xuất hiện bảng thông báo thoái khỏi chương trình sau khi hoàn thành kết nối tới DTB</t>
-  </si>
-  <si>
     <t>Lỗi tạo ra con trỏ 'Pointer.cur'</t>
   </si>
   <si>
-    <t>Chuyển ngay vào bảng nhập tên server</t>
-  </si>
-  <si>
-    <t>Không cho phép nhấn nút 'Test Connection'</t>
-  </si>
-  <si>
-    <t>Không xuất hiện bảng thông báo thoát khỏi chương trình và truy cập ngay vào frmMain</t>
-  </si>
-  <si>
-    <t>Xem lại lỗi</t>
-  </si>
-  <si>
     <t>Vẫn còn lỗi</t>
+  </si>
+  <si>
+    <t>Không xuất hiện lỗi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,27 +215,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,24 +249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -487,112 +424,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="5"/>
-    <col min="2" max="2" width="90.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="90.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="13.8">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="13.8">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="13.8">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" ht="13.8">
       <c r="A6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -604,24 +513,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>